<commit_message>
Code Commit - 10 March 2023
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\603214\Documents\UiPath\TEL_GF_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E37AB9-F910-4551-BB2F-C6FB30F362FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C47FDC6-9DE4-4AE6-B137-A13842F62BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
   <si>
     <t>Name</t>
   </si>
@@ -309,12 +309,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>C:\Box\Personal_603214\External\RAJAT\Development\TSI-GF\Invoices\INV-11008160.pdf</t>
-  </si>
-  <si>
-    <t>InvoicePath</t>
-  </si>
-  <si>
     <t>FilterColumnName</t>
   </si>
   <si>
@@ -369,9 +363,6 @@
     <t>ExcpMsg_MailMissing</t>
   </si>
   <si>
-    <t>Email missing for below invoice number</t>
-  </si>
-  <si>
     <t>ExcpMsg_MailAttachMissing</t>
   </si>
   <si>
@@ -438,10 +429,31 @@
     <t>GF: Process Exceution Failed</t>
   </si>
   <si>
-    <t>Dear User, &lt;br&gt;&lt;br&gt;GF process execution has failed. For more details please see below exception message</t>
-  </si>
-  <si>
     <t>maheshwari.raj@tel.com</t>
+  </si>
+  <si>
+    <t>TempTrackerSheetName</t>
+  </si>
+  <si>
+    <t>StatusTrackerSheetName</t>
+  </si>
+  <si>
+    <t>Dear User, &lt;br&gt;&lt;br&gt;GF process execution has failed. For more details please see below exception message. &lt;br&gt;</t>
+  </si>
+  <si>
+    <t>Required invoice attachment is missing.</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Shared Folder</t>
+  </si>
+  <si>
+    <t>Path.combine(Environment.CurrentDirectory,in_config("StatusTrackerLocalFolder")</t>
   </si>
 </sst>
 </file>
@@ -473,18 +485,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -499,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -515,8 +521,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -834,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -915,39 +919,39 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>137</v>
@@ -955,18 +959,18 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>138</v>
+        <v>128</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>138</v>
+        <v>129</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1963,10 +1967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1009"/>
+  <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2133,7 +2137,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -2170,34 +2174,34 @@
     </row>
     <row r="20" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2256,15 +2260,15 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -2272,225 +2276,240 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" t="s">
         <v>52</v>
       </c>
-      <c r="B35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
         <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+        <v>121</v>
+      </c>
+      <c r="C37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
         <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+        <v>122</v>
+      </c>
+      <c r="C38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
         <v>53</v>
       </c>
       <c r="B39" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1">
+      <c r="C39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
         <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
         <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1">
+        <v>120</v>
+      </c>
+      <c r="C42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="B43" s="7"/>
     </row>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A44" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B45" s="7"/>
-    </row>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1">
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>59</v>
-      </c>
-      <c r="B48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A49" t="s">
         <v>64</v>
       </c>
-      <c r="B49">
+      <c r="B48">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="51" spans="1:2" ht="58">
+    <row r="49" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="50" spans="1:2" ht="58">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.5">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.5">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.5">
-      <c r="A53" t="s">
-        <v>84</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="14.5">
-      <c r="B54" s="6"/>
-    </row>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55">
+        <v>5000</v>
+      </c>
+    </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56">
-        <v>5000</v>
+        <v>75</v>
+      </c>
+      <c r="B56" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B61" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="14.25" customHeight="1">
       <c r="A63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" t="s">
         <v>96</v>
       </c>
-      <c r="B63" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A64" t="s">
-        <v>97</v>
-      </c>
-      <c r="B64" t="s">
+    </row>
+    <row r="64" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A64" s="5" t="s">
         <v>98</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A65" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>112</v>
+        <v>99</v>
+      </c>
+      <c r="B65" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A66" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B66" s="5">
-        <v>10</v>
+        <v>106</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A67" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
@@ -2498,12 +2517,12 @@
         <v>102</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A69" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>104</v>
@@ -2514,21 +2533,32 @@
         <v>105</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A71" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A75" t="s">
+        <v>142</v>
+      </c>
+    </row>
     <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3462,7 +3492,6 @@
     <row r="1006" ht="14.25" customHeight="1"/>
     <row r="1007" ht="14.25" customHeight="1"/>
     <row r="1008" ht="14.25" customHeight="1"/>
-    <row r="1009" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Path Change - 10 March 2023
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\603214\Documents\UiPath\TEL_GF_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C47FDC6-9DE4-4AE6-B137-A13842F62BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6818CC-0268-4BE2-AB92-9798CE22D00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -183,9 +183,6 @@
     <t>ExcpMsg_LoginMissing</t>
   </si>
   <si>
-    <t>TemplateFolder</t>
-  </si>
-  <si>
     <t>Status_TrackerShared</t>
   </si>
   <si>
@@ -384,18 +381,6 @@
     <t>C:\Box\Personal_603214\External\RAJAT\Development\GF\FlatFiles</t>
   </si>
   <si>
-    <t>C:\Users\603214\Documents\UiPath\TEL_GF_Process\Data\Temp\Template\Temp_Tracker.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\603214\Documents\UiPath\TEL_GF_Process\Data\Temp\Temp_Tracker.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\603214\Documents\UiPath\TEL_GF_Process\Data\Temp\Template\Status Tracker.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\603214\Documents\UiPath\TEL_GF_Process\Data\Temp\Status Tracker.xlsx</t>
-  </si>
-  <si>
     <t>EmailSuccessSub</t>
   </si>
   <si>
@@ -450,10 +435,19 @@
     <t>Output</t>
   </si>
   <si>
-    <t>Shared Folder</t>
-  </si>
-  <si>
     <t>Path.combine(Environment.CurrentDirectory,in_config("StatusTrackerLocalFolder")</t>
+  </si>
+  <si>
+    <t>Data\Input\Template\Status Tracker.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Output\Status Tracker.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Input\Template\Temp_Tracker.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Output\Temp_Tracker.xlsx</t>
   </si>
 </sst>
 </file>
@@ -505,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -522,6 +516,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,58 +914,58 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1967,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1008"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:A75"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2137,71 +2132,71 @@
         <v>51</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2244,19 +2239,19 @@
     </row>
     <row r="30" spans="1:3" ht="14.5">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2265,7 +2260,7 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
@@ -2273,83 +2268,95 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
       <c r="B35" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" t="s">
-        <v>139</v>
-      </c>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
         <v>53</v>
       </c>
-      <c r="B39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="B40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
         <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="C41" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
         <v>55</v>
       </c>
-      <c r="B42" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B43" s="7"/>
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B44" s="7"/>
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>58</v>
@@ -2357,208 +2364,185 @@
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>57</v>
-      </c>
-      <c r="B46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="B46" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="58">
       <c r="A48" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="50" spans="1:2" ht="58">
+        <v>79</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.5">
+      <c r="A49" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.5">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="14.5">
-      <c r="A51" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="14.5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="14.5">
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>70</v>
+      </c>
+      <c r="B52" s="7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55">
-        <v>5000</v>
+        <v>76</v>
+      </c>
+      <c r="B55" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A61" t="s">
-        <v>87</v>
-      </c>
-      <c r="B61" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A62" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A61" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A63" t="s">
-        <v>95</v>
-      </c>
-      <c r="B63" t="s">
-        <v>96</v>
+      <c r="B61" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A62" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A63" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A64" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A65" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B65" s="5">
-        <v>10</v>
+        <v>101</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A66" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A67" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A68" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A69" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A70" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A67" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="71" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A71" t="s">
-        <v>135</v>
-      </c>
-      <c r="B71" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A72" t="s">
+      <c r="A71" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B72" t="s">
-        <v>88</v>
-      </c>
-    </row>
+    </row>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="75" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A75" t="s">
-        <v>142</v>
-      </c>
-    </row>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3488,10 +3472,6 @@
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
-    <row r="1005" ht="14.25" customHeight="1"/>
-    <row r="1006" ht="14.25" customHeight="1"/>
-    <row r="1007" ht="14.25" customHeight="1"/>
-    <row r="1008" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes for Service - 13 March 2023
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\603214\Documents\UiPath\TEL_GF_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6818CC-0268-4BE2-AB92-9798CE22D00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E459286-C011-4E49-9926-1A84F065B016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -448,6 +448,27 @@
   </si>
   <si>
     <t>Data\Output\Temp_Tracker.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Box\Personal_603214\External\RAJAT\Development\GF Service Report</t>
+  </si>
+  <si>
+    <t>ServiceReportFolderPath</t>
+  </si>
+  <si>
+    <t>.pdf</t>
+  </si>
+  <si>
+    <t>ServiceReportFileExtension</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>LocalInvoiceFolder</t>
+  </si>
+  <si>
+    <t>Data\Output\Invoices</t>
   </si>
 </sst>
 </file>
@@ -1962,9 +1983,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -2280,269 +2301,293 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" s="5" t="s">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-    </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" t="s">
-        <v>134</v>
-      </c>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
         <v>54</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>140</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B42" s="7"/>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" t="s">
-        <v>56</v>
-      </c>
-    </row>
+        <v>147</v>
+      </c>
+      <c r="C43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A49" t="s">
         <v>58</v>
       </c>
-      <c r="B45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A46" t="s">
+      <c r="B49" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A50" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B50" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="58">
-      <c r="A48" t="s">
+    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="52" spans="1:2" ht="14.5">
+      <c r="A52" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B52" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.5">
-      <c r="A49" t="s">
+    <row r="53" spans="1:2" ht="14.5">
+      <c r="A53" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B53" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.5">
-      <c r="A50" t="s">
+    <row r="54" spans="1:2" ht="14.5">
+      <c r="A54" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="52" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A52" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52" s="7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A53" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A54" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" t="s">
-        <v>73</v>
-      </c>
-    </row>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="B56" s="7">
+        <v>5000</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
       <c r="A60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A64" t="s">
         <v>94</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B64" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A61" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A62" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A63" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A64" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A65" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A67" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A68" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A69" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A70" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B70" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A67" t="s">
+    <row r="71" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
         <v>130</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B71" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A68" t="s">
+    <row r="72" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
         <v>131</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="70" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="71" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A71" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A75" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
     <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3472,6 +3517,10 @@
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
+    <row r="1006" ht="14.25" customHeight="1"/>
+    <row r="1007" ht="14.25" customHeight="1"/>
+    <row r="1008" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>